<commit_message>
added buttons for prediction
</commit_message>
<xml_diff>
--- a/data/Datasets/data_set_after_feature_engineering.xlsx
+++ b/data/Datasets/data_set_after_feature_engineering.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25311"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{344297B8-AC87-4694-8BC8-4D383EBAA678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E347CC2-4218-43B3-8778-5028F1138572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -185,7 +185,7 @@
     <t>bmw x1</t>
   </si>
   <si>
-    <t>Highclass Families</t>
+    <t>Family</t>
   </si>
   <si>
     <t>bmw x3</t>
@@ -305,7 +305,7 @@
     <t>nissan nv200</t>
   </si>
   <si>
-    <t>Upper Middle Class</t>
+    <t>Upper Class</t>
   </si>
   <si>
     <t>nissan teana</t>
@@ -757,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="U15" workbookViewId="0">
+      <selection activeCell="AF32" sqref="AF32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2945,7 +2945,7 @@
         <v>178974</v>
       </c>
       <c r="AE23" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:31">
@@ -3610,7 +3610,7 @@
         <v>133249</v>
       </c>
       <c r="AE30" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:31">
@@ -3705,7 +3705,7 @@
         <v>93159</v>
       </c>
       <c r="AE31" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:31">
@@ -3800,7 +3800,7 @@
         <v>93159</v>
       </c>
       <c r="AE32" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:31">
@@ -4370,7 +4370,7 @@
         <v>135821</v>
       </c>
       <c r="AE38" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:31">
@@ -4655,7 +4655,7 @@
         <v>1276094</v>
       </c>
       <c r="AE41" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:31">
@@ -4845,7 +4845,7 @@
         <v>494904</v>
       </c>
       <c r="AE43" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:31">
@@ -4940,7 +4940,7 @@
         <v>223059</v>
       </c>
       <c r="AE44" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:31">
@@ -5035,7 +5035,7 @@
         <v>76411</v>
       </c>
       <c r="AE45" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:31">
@@ -5320,7 +5320,7 @@
         <v>68590</v>
       </c>
       <c r="AE48" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:31">
@@ -5510,7 +5510,7 @@
         <v>16406</v>
       </c>
       <c r="AE50" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:31">
@@ -5605,7 +5605,7 @@
         <v>8059</v>
       </c>
       <c r="AE51" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:31">
@@ -5795,7 +5795,7 @@
         <v>10755</v>
       </c>
       <c r="AE53" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:31">
@@ -5890,7 +5890,7 @@
         <v>10755</v>
       </c>
       <c r="AE54" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:31">
@@ -6175,7 +6175,7 @@
         <v>892671</v>
       </c>
       <c r="AE57" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="58" spans="1:31">
@@ -6460,7 +6460,7 @@
         <v>428567</v>
       </c>
       <c r="AE60" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:31">
@@ -6555,7 +6555,7 @@
         <v>428567</v>
       </c>
       <c r="AE61" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="62" spans="1:31">
@@ -6745,7 +6745,7 @@
         <v>428567</v>
       </c>
       <c r="AE63" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:31">
@@ -6840,7 +6840,7 @@
         <v>428567</v>
       </c>
       <c r="AE64" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:31">
@@ -6935,7 +6935,7 @@
         <v>428567</v>
       </c>
       <c r="AE65" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="66" spans="1:31">
@@ -7030,7 +7030,7 @@
         <v>428567</v>
       </c>
       <c r="AE66" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>